<commit_message>
updated link files, removing plots
</commit_message>
<xml_diff>
--- a/inputs/190905_data_from_RTS.xlsx
+++ b/inputs/190905_data_from_RTS.xlsx
@@ -370,7 +370,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="39:43 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -421,7 +421,7 @@
   <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="39:43"/>
+      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1557,7 +1557,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="39:43"/>
+      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2658,17 +2658,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="39:43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="35.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="22.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="3" style="4" width="13.55"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="8" min="3" style="4" width="13.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="4" width="8.72"/>
   </cols>
   <sheetData>
@@ -2706,7 +2706,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -2731,8 +2731,12 @@
       <c r="H4" s="10" t="n">
         <v>293020.90974</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I4" s="4" t="n">
+        <f aca="false">SUM(C4:H4)</f>
+        <v>1661010.23214239</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -2757,8 +2761,12 @@
       <c r="H5" s="10" t="n">
         <v>34937.913107</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I5" s="4" t="n">
+        <f aca="false">SUM(C5:H5)</f>
+        <v>201548.138033112</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -2783,8 +2791,12 @@
       <c r="H6" s="10" t="n">
         <v>8030.000972</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I6" s="4" t="n">
+        <f aca="false">SUM(C6:H6)</f>
+        <v>48898.2449546822</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -2809,8 +2821,12 @@
       <c r="H7" s="10" t="n">
         <v>13307.255285</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I7" s="4" t="n">
+        <f aca="false">SUM(C7:H7)</f>
+        <v>78916.5731890088</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -2835,8 +2851,12 @@
       <c r="H8" s="10" t="n">
         <v>9739.533989</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I8" s="4" t="n">
+        <f aca="false">SUM(C8:H8)</f>
+        <v>62574.8499484766</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
@@ -2861,8 +2881,12 @@
       <c r="H9" s="10" t="n">
         <v>563956.946829</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I9" s="4" t="n">
+        <f aca="false">SUM(C9:H9)</f>
+        <v>3406313.40232377</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
@@ -2887,8 +2911,12 @@
       <c r="H10" s="10" t="n">
         <v>30349.930283</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I10" s="4" t="n">
+        <f aca="false">SUM(C10:H10)</f>
+        <v>193596.384289182</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
@@ -2913,8 +2941,12 @@
       <c r="H11" s="10" t="n">
         <v>4075.542225</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I11" s="4" t="n">
+        <f aca="false">SUM(C11:H11)</f>
+        <v>25230.1630287865</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
@@ -2939,8 +2971,12 @@
       <c r="H12" s="10" t="n">
         <v>123612.902261</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I12" s="4" t="n">
+        <f aca="false">SUM(C12:H12)</f>
+        <v>784586.870195978</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
@@ -2965,8 +3001,12 @@
       <c r="H13" s="10" t="n">
         <v>69320.053272</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I13" s="4" t="n">
+        <f aca="false">SUM(C13:H13)</f>
+        <v>447956.605961681</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
@@ -2991,8 +3031,12 @@
       <c r="H14" s="10" t="n">
         <v>161388.749511</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I14" s="4" t="n">
+        <f aca="false">SUM(C14:H14)</f>
+        <v>945719.237515719</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
@@ -3017,8 +3061,12 @@
       <c r="H15" s="10" t="n">
         <v>50128.861514</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I15" s="4" t="n">
+        <f aca="false">SUM(C15:H15)</f>
+        <v>297566.731491305</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
         <v>13</v>
       </c>
@@ -3043,8 +3091,12 @@
       <c r="H16" s="10" t="n">
         <v>2462.052487</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I16" s="4" t="n">
+        <f aca="false">SUM(C16:H16)</f>
+        <v>15205.5002479038</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
         <v>13</v>
       </c>
@@ -3069,8 +3121,12 @@
       <c r="H17" s="10" t="n">
         <v>87734.475017</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I17" s="4" t="n">
+        <f aca="false">SUM(C17:H17)</f>
+        <v>534415.247632041</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
@@ -3095,8 +3151,12 @@
       <c r="H18" s="10" t="n">
         <v>40500.48414</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I18" s="4" t="n">
+        <f aca="false">SUM(C18:H18)</f>
+        <v>262396.111764686</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
         <v>14</v>
       </c>
@@ -3121,8 +3181,12 @@
       <c r="H19" s="10" t="n">
         <v>258475.9284</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I19" s="4" t="n">
+        <f aca="false">SUM(C19:H19)</f>
+        <v>1379091.3906878</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
         <v>14</v>
       </c>
@@ -3147,8 +3211,12 @@
       <c r="H20" s="10" t="n">
         <v>40404.858191</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I20" s="4" t="n">
+        <f aca="false">SUM(C20:H20)</f>
+        <v>218079.459849148</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
         <v>14</v>
       </c>
@@ -3173,8 +3241,12 @@
       <c r="H21" s="10" t="n">
         <v>2392.62074</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I21" s="4" t="n">
+        <f aca="false">SUM(C21:H21)</f>
+        <v>14673.8962322646</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
         <v>14</v>
       </c>
@@ -3199,8 +3271,12 @@
       <c r="H22" s="10" t="n">
         <v>648083.239268</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I22" s="4" t="n">
+        <f aca="false">SUM(C22:H22)</f>
+        <v>3850560.64148056</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
         <v>14</v>
       </c>
@@ -3225,8 +3301,12 @@
       <c r="H23" s="10" t="n">
         <v>98113.469888</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I23" s="4" t="n">
+        <f aca="false">SUM(C23:H23)</f>
+        <v>644461.943098083</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
         <v>15</v>
       </c>
@@ -3251,8 +3331,12 @@
       <c r="H24" s="10" t="n">
         <v>97761.161283</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I24" s="4" t="n">
+        <f aca="false">SUM(C24:H24)</f>
+        <v>574314.618275562</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
         <v>15</v>
       </c>
@@ -3277,8 +3361,12 @@
       <c r="H25" s="10" t="n">
         <v>165742.259726</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I25" s="4" t="n">
+        <f aca="false">SUM(C25:H25)</f>
+        <v>961456.957470249</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
         <v>15</v>
       </c>
@@ -3303,8 +3391,12 @@
       <c r="H26" s="10" t="n">
         <v>16833.04663</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I26" s="4" t="n">
+        <f aca="false">SUM(C26:H26)</f>
+        <v>102680.342993817</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
         <v>15</v>
       </c>
@@ -3329,8 +3421,12 @@
       <c r="H27" s="10" t="n">
         <v>75128.713078</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I27" s="4" t="n">
+        <f aca="false">SUM(C27:H27)</f>
+        <v>471956.15833222</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
         <v>15</v>
       </c>
@@ -3355,8 +3451,12 @@
       <c r="H28" s="10" t="n">
         <v>31427.066686</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I28" s="4" t="n">
+        <f aca="false">SUM(C28:H28)</f>
+        <v>203942.61088828</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
         <v>16</v>
       </c>
@@ -3381,8 +3481,12 @@
       <c r="H29" s="10" t="n">
         <v>448302.727469</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I29" s="4" t="n">
+        <f aca="false">SUM(C29:H29)</f>
+        <v>2580235.03362475</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
         <v>16</v>
       </c>
@@ -3407,8 +3511,12 @@
       <c r="H30" s="10" t="n">
         <v>80416.898978</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I30" s="4" t="n">
+        <f aca="false">SUM(C30:H30)</f>
+        <v>460560.48264908</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
         <v>16</v>
       </c>
@@ -3433,8 +3541,12 @@
       <c r="H31" s="10" t="n">
         <v>20958.144259</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I31" s="4" t="n">
+        <f aca="false">SUM(C31:H31)</f>
+        <v>126886.412984617</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
         <v>16</v>
       </c>
@@ -3459,8 +3571,12 @@
       <c r="H32" s="10" t="n">
         <v>35247.454327</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I32" s="4" t="n">
+        <f aca="false">SUM(C32:H32)</f>
+        <v>218207.870275656</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
         <v>16</v>
       </c>
@@ -3485,8 +3601,12 @@
       <c r="H33" s="10" t="n">
         <v>15621.719387</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I33" s="4" t="n">
+        <f aca="false">SUM(C33:H33)</f>
+        <v>101650.866869427</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
         <v>17</v>
       </c>
@@ -3511,8 +3631,12 @@
       <c r="H34" s="10" t="n">
         <v>444186.503952</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I34" s="4" t="n">
+        <f aca="false">SUM(C34:H34)</f>
+        <v>2334434.43207284</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
         <v>17</v>
       </c>
@@ -3537,8 +3661,12 @@
       <c r="H35" s="10" t="n">
         <v>29978.696947</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I35" s="4" t="n">
+        <f aca="false">SUM(C35:H35)</f>
+        <v>140575.805521435</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
         <v>17</v>
       </c>
@@ -3563,8 +3691,12 @@
       <c r="H36" s="10" t="n">
         <v>3148.680046</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I36" s="4" t="n">
+        <f aca="false">SUM(C36:H36)</f>
+        <v>19207.5036037171</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
         <v>17</v>
       </c>
@@ -3589,8 +3721,12 @@
       <c r="H37" s="10" t="n">
         <v>138754.602761</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I37" s="4" t="n">
+        <f aca="false">SUM(C37:H37)</f>
+        <v>774657.449059165</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
         <v>17</v>
       </c>
@@ -3615,8 +3751,12 @@
       <c r="H38" s="10" t="n">
         <v>67448.129857</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I38" s="4" t="n">
+        <f aca="false">SUM(C38:H38)</f>
+        <v>433673.702981316</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
         <v>18</v>
       </c>
@@ -3641,8 +3781,12 @@
       <c r="H39" s="10" t="n">
         <v>700681.100222</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I39" s="4" t="n">
+        <f aca="false">SUM(C39:H39)</f>
+        <v>3610916.39576586</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
         <v>18</v>
       </c>
@@ -3667,8 +3811,12 @@
       <c r="H40" s="10" t="n">
         <v>83843.135724</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I40" s="4" t="n">
+        <f aca="false">SUM(C40:H40)</f>
+        <v>688900.398953522</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
         <v>18</v>
       </c>
@@ -3693,8 +3841,12 @@
       <c r="H41" s="10" t="n">
         <v>14378.194802</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I41" s="4" t="n">
+        <f aca="false">SUM(C41:H41)</f>
+        <v>89421.0638985703</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
         <v>18</v>
       </c>
@@ -3719,8 +3871,12 @@
       <c r="H42" s="10" t="n">
         <v>105452.564072</v>
       </c>
-    </row>
-    <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I42" s="4" t="n">
+        <f aca="false">SUM(C42:H42)</f>
+        <v>603676.825914675</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
         <v>18</v>
       </c>
@@ -3744,6 +3900,10 @@
       </c>
       <c r="H43" s="10" t="n">
         <v>48647.147616</v>
+      </c>
+      <c r="I43" s="4" t="n">
+        <f aca="false">SUM(C43:H43)</f>
+        <v>316061.72894669</v>
       </c>
     </row>
   </sheetData>
@@ -3765,7 +3925,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="1" sqref="39:43 D22"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>